<commit_message>
some changes for a new release
</commit_message>
<xml_diff>
--- a/mybook.xlsx
+++ b/mybook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Felix/DEV/release-excel-workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BCE08A-C1BF-D74B-8F2E-2FCABCB0A5C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE953AC-E9E7-DF41-AE0D-77AEC991B08E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="17540" xr2:uid="{D67E1A77-79FF-B24A-8C47-6599F423D796}"/>
   </bookViews>
@@ -30,6 +30,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>some changes for a new release</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,8 +415,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>2</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>